<commit_message>
Add 'width' and 'height' parameters
</commit_message>
<xml_diff>
--- a/uploads/form-2_mz.xlsx
+++ b/uploads/form-2_mz.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t xml:space="preserve">&lt;ORGANIZATION_FULL_NAME&gt;</t>
   </si>
@@ -63,6 +63,9 @@
     <t xml:space="preserve">Наименование</t>
   </si>
   <si>
+    <t xml:space="preserve">Серия лекарственного средства</t>
+  </si>
+  <si>
     <t xml:space="preserve">Источник финансирования</t>
   </si>
   <si>
@@ -99,7 +102,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -142,6 +145,14 @@
     <font>
       <i val="true"/>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -212,7 +223,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -238,6 +249,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -249,11 +264,15 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -265,23 +284,27 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -302,24 +325,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G31" activeCellId="0" sqref="G31"/>
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="46.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="17.92"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="4" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.16"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="14.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="3" width="17.92"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14.16"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="14.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="16.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -327,132 +350,142 @@
         <v>0</v>
       </c>
       <c r="B1" s="5"/>
-      <c r="G1" s="6"/>
+      <c r="C1" s="6"/>
       <c r="H1" s="7"/>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="8"/>
+      <c r="J1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="7"/>
+      <c r="K1" s="8"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="H2" s="7"/>
       <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="10"/>
+      <c r="H3" s="7"/>
       <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="H4" s="7"/>
       <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
     </row>
     <row r="5" customFormat="false" ht="22.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
+      <c r="H5" s="7"/>
       <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-    </row>
-    <row r="6" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="10" t="s">
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+    </row>
+    <row r="6" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-    </row>
-    <row r="7" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="12" t="s">
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+    </row>
+    <row r="7" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="H8" s="14"/>
-      <c r="J8" s="15" t="s">
+      <c r="C8" s="16"/>
+      <c r="I8" s="17"/>
+      <c r="K8" s="18" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" s="17" customFormat="true" ht="51.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="16" t="s">
+    <row r="9" s="20" customFormat="true" ht="51.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="E9" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="16" t="s">
+      <c r="F9" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="G9" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="H9" s="16" t="s">
+      <c r="H9" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="I9" s="16" t="s">
+      <c r="I9" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="J9" s="16" t="s">
+      <c r="J9" s="19" t="s">
         <v>18</v>
+      </c>
+      <c r="K9" s="19" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="A1:B2"/>
-    <mergeCell ref="I1:J5"/>
+    <mergeCell ref="J1:K5"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A6:J6"/>
-    <mergeCell ref="A7:J7"/>
+    <mergeCell ref="A6:K6"/>
+    <mergeCell ref="A7:K7"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.39375" right="0.196527777777778" top="0.196527777777778" bottom="0.307638888888889" header="0.511805555555555" footer="0.196527777777778"/>

</xml_diff>